<commit_message>
add report for cloud lab1
</commit_message>
<xml_diff>
--- a/cloud/lab1/Mapping Rules AWS team 3.xlsx
+++ b/cloud/lab1/Mapping Rules AWS team 3.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D632191-7F28-4646-AF69-29185E0EADEB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF397BC-FED4-41B1-9966-41E086DA9B71}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="141">
   <si>
     <t>IT Tower</t>
   </si>
@@ -842,8 +842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F456EB8C-FCFA-4ECE-9DD9-04F2A23D9C0E}">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" zoomScale="64" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>